<commit_message>
State updates; removed boundary penalty. Re-ran Iters 2-4.
</commit_message>
<xml_diff>
--- a/lab5/Metrics_Summary.xlsx
+++ b/lab5/Metrics_Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\ML Python Notebooks\CS8321_Labs\lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9126197-BF0B-40A4-A11A-790994D4825D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E68820-A14F-4EBD-9878-4CF90AA70AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9577D97A-D947-4A78-8DCC-F05C39BECA70}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{9577D97A-D947-4A78-8DCC-F05C39BECA70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Num2Move = 1 (best result)</t>
-  </si>
-  <si>
     <t>Metrics</t>
   </si>
   <si>
@@ -81,13 +78,16 @@
   </si>
   <si>
     <t>Sum of all rewards for all steps</t>
+  </si>
+  <si>
+    <t>Need to re-verify Num2Move</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,13 +103,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -139,31 +153,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,11 +522,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903B1E1A-DDE3-4145-97CC-64135EF045FE}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -514,193 +538,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="6">
         <v>118</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="6">
         <v>12.74</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>3.19</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="6">
         <v>10007.549999999999</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="6">
         <v>122.56</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
-        <v>168.12</v>
-      </c>
-      <c r="C3" s="4">
-        <v>23.07</v>
-      </c>
-      <c r="D3" s="4">
-        <v>10.88</v>
-      </c>
-      <c r="E3" s="4">
-        <v>11201.42</v>
-      </c>
-      <c r="F3" s="4">
-        <v>-0.6</v>
-      </c>
-      <c r="G3" s="3"/>
+      <c r="B3" s="15">
+        <v>165.41</v>
+      </c>
+      <c r="C3" s="15">
+        <v>17.66</v>
+      </c>
+      <c r="D3" s="15">
+        <v>6.5</v>
+      </c>
+      <c r="E3" s="15">
+        <v>12100.01</v>
+      </c>
+      <c r="F3" s="15">
+        <v>-1.56</v>
+      </c>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
-        <v>132.55000000000001</v>
-      </c>
-      <c r="C4" s="4">
-        <v>15</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1.84</v>
-      </c>
-      <c r="E4" s="4">
-        <v>7865.31</v>
-      </c>
-      <c r="F4" s="4">
-        <v>-1279.99</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="B4" s="15">
+        <v>293.02</v>
+      </c>
+      <c r="C4" s="15">
+        <v>30.49</v>
+      </c>
+      <c r="D4" s="15">
+        <v>25.98</v>
+      </c>
+      <c r="E4" s="15">
+        <v>8369.94</v>
+      </c>
+      <c r="F4" s="15">
+        <v>1172.07</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>132.44999999999999</v>
+      </c>
+      <c r="C5" s="6">
+        <v>14.05</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="E5" s="6">
+        <v>8083.11</v>
+      </c>
+      <c r="F5" s="6">
+        <v>112.67</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="B8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="11">
-        <v>108.35</v>
-      </c>
-      <c r="C5" s="11">
-        <v>12.37</v>
-      </c>
-      <c r="D5" s="11">
-        <v>1.58</v>
-      </c>
-      <c r="E5" s="11">
-        <v>7457.85</v>
-      </c>
-      <c r="F5" s="11">
-        <v>-533.29999999999995</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -712,5 +754,6 @@
     <mergeCell ref="B9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
datasets with tweaked reward approach for boundary conditions
</commit_message>
<xml_diff>
--- a/lab5/Metrics_Summary.xlsx
+++ b/lab5/Metrics_Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\ML Python Notebooks\CS8321_Labs\lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E68820-A14F-4EBD-9878-4CF90AA70AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC782E19-8E20-4A7F-B04B-AB2B4F83D34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{9577D97A-D947-4A78-8DCC-F05C39BECA70}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9577D97A-D947-4A78-8DCC-F05C39BECA70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,14 +80,17 @@
     <t>Sum of all rewards for all steps</t>
   </si>
   <si>
-    <t>Need to re-verify Num2Move</t>
+    <t>Num2Move = 1; Discount of -1 for "far out" movements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,8 +114,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +134,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -153,25 +177,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -185,7 +202,59 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,226 +592,226 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="16" customWidth="1"/>
+    <col min="7" max="7" width="49.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="30" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="17">
         <v>118</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="18">
         <v>12.74</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="19">
         <v>3.19</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="20">
         <v>10007.549999999999</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="20">
         <v>122.56</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="20">
         <v>165.41</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="19">
         <v>17.66</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="19">
         <v>6.5</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="21">
         <v>12100.01</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="21">
         <v>-1.56</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="15">
-        <v>293.02</v>
-      </c>
-      <c r="C4" s="15">
-        <v>30.49</v>
-      </c>
-      <c r="D4" s="15">
-        <v>25.98</v>
-      </c>
-      <c r="E4" s="15">
-        <v>8369.94</v>
-      </c>
-      <c r="F4" s="15">
-        <v>1172.07</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="B4" s="21">
+        <v>219.84</v>
+      </c>
+      <c r="C4" s="22">
+        <v>19.940000000000001</v>
+      </c>
+      <c r="D4" s="22">
+        <v>6.74</v>
+      </c>
+      <c r="E4" s="20">
+        <v>8490.4</v>
+      </c>
+      <c r="F4" s="17">
+        <v>182.86</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
-        <v>132.44999999999999</v>
-      </c>
-      <c r="C5" s="6">
-        <v>14.05</v>
-      </c>
-      <c r="D5" s="6">
-        <v>2.4</v>
-      </c>
-      <c r="E5" s="6">
-        <v>8083.11</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="B5" s="23">
+        <v>129.19</v>
+      </c>
+      <c r="C5" s="24">
+        <v>13.7</v>
+      </c>
+      <c r="D5" s="25">
+        <v>2.38</v>
+      </c>
+      <c r="E5" s="26">
+        <v>7740.5</v>
+      </c>
+      <c r="F5" s="23">
         <v>112.67</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
additional runs for iters 3 & 4
</commit_message>
<xml_diff>
--- a/lab5/Metrics_Summary.xlsx
+++ b/lab5/Metrics_Summary.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\ML Python Notebooks\CS8321_Labs\lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC782E19-8E20-4A7F-B04B-AB2B4F83D34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585CD73A-AF03-4AF0-98C3-5CFCEC1D1D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9577D97A-D947-4A78-8DCC-F05C39BECA70}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{9577D97A-D947-4A78-8DCC-F05C39BECA70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
   <si>
     <t>Iteration</t>
   </si>
@@ -81,6 +82,21 @@
   </si>
   <si>
     <t>Num2Move = 1; Discount of -1 for "far out" movements</t>
+  </si>
+  <si>
+    <t>Num2Move = 1; Discount of 0 for "far out" movements</t>
+  </si>
+  <si>
+    <t>Num2Move = 1; Discount of -1 for "far out" movements and -1 for "too close" movements</t>
+  </si>
+  <si>
+    <t>4a</t>
+  </si>
+  <si>
+    <t>4b</t>
+  </si>
+  <si>
+    <t>iter4a_1_bvm1_corr_results10000a</t>
   </si>
 </sst>
 </file>
@@ -177,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -197,12 +213,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -253,6 +263,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -592,226 +633,226 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="16" customWidth="1"/>
-    <col min="7" max="7" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="49.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="15">
         <v>118</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="16">
         <v>12.74</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="17">
         <v>3.19</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="18">
         <v>10007.549999999999</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="18">
         <v>122.56</v>
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="18">
         <v>165.41</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="17">
         <v>17.66</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="17">
         <v>6.5</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="19">
         <v>12100.01</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="19">
         <v>-1.56</v>
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="19">
         <v>219.84</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="20">
         <v>19.940000000000001</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="20">
         <v>6.74</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="18">
         <v>8490.4</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="15">
         <v>182.86</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="21">
         <v>129.19</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="22">
         <v>13.7</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="23">
         <v>2.38</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="24">
         <v>7740.5</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="21">
         <v>112.67</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -825,4 +866,275 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DEF4F7-9574-461C-B23E-246C0AB59C8D}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="49.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36">
+        <v>118</v>
+      </c>
+      <c r="C2" s="37">
+        <v>12.74</v>
+      </c>
+      <c r="D2" s="37">
+        <v>3.19</v>
+      </c>
+      <c r="E2" s="36">
+        <v>10007.549999999999</v>
+      </c>
+      <c r="F2" s="36">
+        <v>122.56</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="36">
+        <v>165.41</v>
+      </c>
+      <c r="C3" s="37">
+        <v>17.66</v>
+      </c>
+      <c r="D3" s="37">
+        <v>6.5</v>
+      </c>
+      <c r="E3" s="36">
+        <v>12100.01</v>
+      </c>
+      <c r="F3" s="36">
+        <v>-1.56</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="36">
+        <v>219.84</v>
+      </c>
+      <c r="C4" s="37">
+        <v>19.940000000000001</v>
+      </c>
+      <c r="D4" s="37">
+        <v>6.74</v>
+      </c>
+      <c r="E4" s="36">
+        <v>8490.4</v>
+      </c>
+      <c r="F4" s="15">
+        <v>182.86</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="38">
+        <v>129.19</v>
+      </c>
+      <c r="C5" s="39">
+        <v>13.7</v>
+      </c>
+      <c r="D5" s="39">
+        <v>2.38</v>
+      </c>
+      <c r="E5" s="38">
+        <v>7740.5</v>
+      </c>
+      <c r="F5" s="38">
+        <v>112.67</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="34">
+        <v>114</v>
+      </c>
+      <c r="C6" s="31">
+        <v>12.78</v>
+      </c>
+      <c r="D6" s="35">
+        <v>1.67</v>
+      </c>
+      <c r="E6" s="32">
+        <v>7053.31</v>
+      </c>
+      <c r="F6" s="34">
+        <v>66.19</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="32">
+        <v>113</v>
+      </c>
+      <c r="C7" s="35">
+        <v>13.04</v>
+      </c>
+      <c r="D7" s="31">
+        <v>1.56</v>
+      </c>
+      <c r="E7" s="34">
+        <v>8068.57</v>
+      </c>
+      <c r="F7" s="34">
+        <v>68.67</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>